<commit_message>
Updating to last version
Better metadata, especially for fungal studies
</commit_message>
<xml_diff>
--- a/olive_FMBN/extra_metadata_FMBN_B.xlsx
+++ b/olive_FMBN/extra_metadata_FMBN_B.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eugenio/Desktop/sviluppo_Metaolive_FMBN/september_2024/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/SAN_DISK_EP/review_metatax_olive/oliveFMBN/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBAF785B-3C1F-8C4A-8856-8437D28ED4A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{28C92D58-4E9B-DA49-BEC0-72F1495CDA82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4680" yWindow="1160" windowWidth="33720" windowHeight="18260" xr2:uid="{CFD21462-16E7-FF4B-8024-48F54831448A}"/>
   </bookViews>
@@ -9045,10 +9045,10 @@
   <dimension ref="A1:T500"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="K414" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="K464" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P413" sqref="P413:P419"/>
+      <selection pane="bottomRight" activeCell="D477" sqref="D477"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -35918,7 +35918,7 @@
         <v>1134</v>
       </c>
       <c r="L435" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M435" t="s">
         <v>239</v>
@@ -35980,7 +35980,7 @@
         <v>1134</v>
       </c>
       <c r="L436" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M436" t="s">
         <v>239</v>
@@ -36042,7 +36042,7 @@
         <v>1134</v>
       </c>
       <c r="L437" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M437" t="s">
         <v>239</v>
@@ -36104,7 +36104,7 @@
         <v>1134</v>
       </c>
       <c r="L438" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M438" t="s">
         <v>239</v>
@@ -36166,7 +36166,7 @@
         <v>1134</v>
       </c>
       <c r="L439" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M439" t="s">
         <v>239</v>
@@ -36228,7 +36228,7 @@
         <v>1134</v>
       </c>
       <c r="L440" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M440" t="s">
         <v>239</v>
@@ -36290,7 +36290,7 @@
         <v>1134</v>
       </c>
       <c r="L441" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M441" t="s">
         <v>239</v>
@@ -36352,7 +36352,7 @@
         <v>1134</v>
       </c>
       <c r="L442" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M442" t="s">
         <v>239</v>
@@ -36414,7 +36414,7 @@
         <v>1134</v>
       </c>
       <c r="L443" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M443" t="s">
         <v>239</v>
@@ -36476,7 +36476,7 @@
         <v>1134</v>
       </c>
       <c r="L444" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M444" t="s">
         <v>239</v>
@@ -36538,7 +36538,7 @@
         <v>1134</v>
       </c>
       <c r="L445" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M445" t="s">
         <v>239</v>
@@ -36600,7 +36600,7 @@
         <v>1134</v>
       </c>
       <c r="L446" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M446" t="s">
         <v>239</v>
@@ -36662,7 +36662,7 @@
         <v>1134</v>
       </c>
       <c r="L447" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M447" t="s">
         <v>239</v>
@@ -36724,7 +36724,7 @@
         <v>1134</v>
       </c>
       <c r="L448" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M448" t="s">
         <v>239</v>
@@ -36786,7 +36786,7 @@
         <v>1134</v>
       </c>
       <c r="L449" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M449" t="s">
         <v>239</v>
@@ -36848,7 +36848,7 @@
         <v>1134</v>
       </c>
       <c r="L450" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M450" t="s">
         <v>239</v>
@@ -36910,7 +36910,7 @@
         <v>1134</v>
       </c>
       <c r="L451" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M451" t="s">
         <v>239</v>
@@ -36972,7 +36972,7 @@
         <v>1134</v>
       </c>
       <c r="L452" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M452" t="s">
         <v>239</v>
@@ -37034,7 +37034,7 @@
         <v>1134</v>
       </c>
       <c r="L453" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M453" t="s">
         <v>239</v>
@@ -37096,7 +37096,7 @@
         <v>1134</v>
       </c>
       <c r="L454" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M454" t="s">
         <v>239</v>
@@ -37158,7 +37158,7 @@
         <v>1134</v>
       </c>
       <c r="L455" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M455" t="s">
         <v>239</v>
@@ -37220,7 +37220,7 @@
         <v>1134</v>
       </c>
       <c r="L456" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M456" t="s">
         <v>239</v>
@@ -37282,7 +37282,7 @@
         <v>1134</v>
       </c>
       <c r="L457" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M457" t="s">
         <v>239</v>
@@ -37344,7 +37344,7 @@
         <v>1134</v>
       </c>
       <c r="L458" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M458" t="s">
         <v>239</v>
@@ -37406,7 +37406,7 @@
         <v>1134</v>
       </c>
       <c r="L459" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M459" t="s">
         <v>239</v>
@@ -37468,7 +37468,7 @@
         <v>1134</v>
       </c>
       <c r="L460" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M460" t="s">
         <v>239</v>
@@ -37530,7 +37530,7 @@
         <v>1134</v>
       </c>
       <c r="L461" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M461" t="s">
         <v>239</v>
@@ -37592,7 +37592,7 @@
         <v>1134</v>
       </c>
       <c r="L462" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M462" t="s">
         <v>239</v>
@@ -37654,7 +37654,7 @@
         <v>1134</v>
       </c>
       <c r="L463" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M463" t="s">
         <v>239</v>
@@ -37716,7 +37716,7 @@
         <v>1134</v>
       </c>
       <c r="L464" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M464" t="s">
         <v>239</v>
@@ -37778,7 +37778,7 @@
         <v>1134</v>
       </c>
       <c r="L465" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M465" t="s">
         <v>239</v>
@@ -37840,7 +37840,7 @@
         <v>1134</v>
       </c>
       <c r="L466" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M466" t="s">
         <v>239</v>
@@ -37902,7 +37902,7 @@
         <v>1134</v>
       </c>
       <c r="L467" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M467" t="s">
         <v>239</v>
@@ -37964,7 +37964,7 @@
         <v>1134</v>
       </c>
       <c r="L468" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M468" t="s">
         <v>239</v>
@@ -38026,7 +38026,7 @@
         <v>1134</v>
       </c>
       <c r="L469" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M469" t="s">
         <v>239</v>
@@ -38088,7 +38088,7 @@
         <v>1134</v>
       </c>
       <c r="L470" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M470" t="s">
         <v>239</v>
@@ -38150,7 +38150,7 @@
         <v>1134</v>
       </c>
       <c r="L471" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M471" t="s">
         <v>239</v>
@@ -38212,7 +38212,7 @@
         <v>1134</v>
       </c>
       <c r="L472" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M472" t="s">
         <v>239</v>
@@ -38274,7 +38274,7 @@
         <v>1134</v>
       </c>
       <c r="L473" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M473" t="s">
         <v>239</v>
@@ -38336,7 +38336,7 @@
         <v>1134</v>
       </c>
       <c r="L474" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M474" t="s">
         <v>239</v>
@@ -38398,7 +38398,7 @@
         <v>1134</v>
       </c>
       <c r="L475" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M475" t="s">
         <v>239</v>
@@ -38460,7 +38460,7 @@
         <v>1134</v>
       </c>
       <c r="L476" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M476" t="s">
         <v>239</v>
@@ -38522,7 +38522,7 @@
         <v>1134</v>
       </c>
       <c r="L477" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M477" t="s">
         <v>239</v>
@@ -38584,7 +38584,7 @@
         <v>1134</v>
       </c>
       <c r="L478" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M478" t="s">
         <v>239</v>
@@ -38646,7 +38646,7 @@
         <v>1134</v>
       </c>
       <c r="L479" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M479" t="s">
         <v>239</v>
@@ -38708,7 +38708,7 @@
         <v>1134</v>
       </c>
       <c r="L480" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M480" t="s">
         <v>239</v>
@@ -38770,7 +38770,7 @@
         <v>1134</v>
       </c>
       <c r="L481" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M481" t="s">
         <v>239</v>
@@ -38832,7 +38832,7 @@
         <v>1134</v>
       </c>
       <c r="L482" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M482" t="s">
         <v>239</v>

</xml_diff>